<commit_message>
1.  Barcelone RDA presentations.  2.  Latest CMIP6 experiment documents / config ...etc.
</commit_message>
<xml_diff>
--- a/cmip6/models/spreadsheet/model-defaults.xlsx
+++ b/cmip6/models/spreadsheet/model-defaults.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="17500" yWindow="5240" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ES-DOC CMIP6 Model Defaults " sheetId="1" r:id="rId1"/>
@@ -197,11 +197,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="16433800" cy="4140200"/>
+    <xdr:ext cx="16395700" cy="4584700"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -209,8 +209,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="50800" y="38100"/>
-          <a:ext cx="16433800" cy="4140200"/>
+          <a:off x="88900" y="38100"/>
+          <a:ext cx="16395700" cy="4584700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -243,7 +243,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike">
+            <a:rPr lang="en-US" sz="2000" b="1" i="0" u="sng" strike="noStrike">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -254,7 +254,7 @@
             </a:rPr>
             <a:t>ES-DOC CMIP6 Model Defaults</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1800">
+          <a:endParaRPr lang="en-US" sz="2000" u="sng">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
@@ -350,6 +350,18 @@
             <a:t> identified which realms are simulated from the following WCRP CMIP6 CV file: </a:t>
           </a:r>
           <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="sng" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>http://bit.ly/2qv1ODS</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -359,7 +371,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>http://bit.ly/2qv1ODS.</a:t>
+            <a:t>.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
@@ -388,16 +400,16 @@
             <a:t>2.  For </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>each</a:t>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="sng" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>each simulated realm</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
@@ -409,19 +421,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> simulated realm please specify whether:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
+            <a:t> specify whether:</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:r>
@@ -446,31 +447,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>  You will document the realm </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="sng" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>from scratch</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>;</a:t>
+            <a:t>  You will start the documentation from new;</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -513,7 +490,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>E.G.  From-Scratch</a:t>
+            <a:t>E.G.  From-New</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -536,7 +513,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>	2.2  You will seed from existing CMIP5 documentation by entering: CMIP5 [model-name].</a:t>
+            <a:t>	2.2  You will start the documentation based upon </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="sng" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>existing CMIP5</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> documentation by entering: CMIP5 [model-name].</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -576,7 +577,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>	2.3  You will seed from a sibling CMIP6 model by entering: CMIP6 [source-id]</a:t>
+            <a:t>	2.3  You will start the documentation from a </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="sng" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>sibling CMIP6 model</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> by entering: CMIP6 [source-id]</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400">
             <a:solidFill>
@@ -662,15 +687,32 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3.  For each simulated realm please specify the name that will be used in the rest of the documentation.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
+            <a:t>3.  For </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="sng" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>each simulated realm</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> please also specify:</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -691,16 +733,109 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>5.  Once completed, ES-DOC requires this information to be either returned via email to </a:t>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	3.1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> T</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>he name that will be used in the rest of the documentation.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4.  Once completed, ES-DOC requires this information either: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	4.1  Via email to </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
@@ -712,19 +847,50 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>david.hassell@ncas.ac.uk</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> or alternatively it can be commited directly to your institutes' official ES-DOC GitHub repository.</a:t>
+            <a:t>david.hassell@ncas.ac.uk;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	4.2 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Or by commiting directly to your institutes' official ES-DOC GitHub repository @ https://github.com/ES-DOC-INSTITUTIONAL.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1600">
             <a:solidFill>
@@ -1005,7 +1171,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,7 +1180,7 @@
     <col min="2" max="9" width="24" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="348" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:9" ht="372" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>

</xml_diff>